<commit_message>
Added test case and fixed bug in compact children method.
</commit_message>
<xml_diff>
--- a/reference/ATest/ATest.xlsx
+++ b/reference/ATest/ATest.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">First Name (OL)</t>
   </si>
   <si>
+    <t xml:space="preserve">Family Letter</t>
+  </si>
+  <si>
     <t xml:space="preserve">Last Name</t>
   </si>
   <si>
@@ -68,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">as</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
   </si>
   <si>
     <t xml:space="preserve">s</t>
@@ -95,7 +101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -124,6 +130,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -180,12 +192,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -282,27 +298,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L1048576"/>
+  <dimension ref="A1:M806"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="13" style="0" width="11.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="5.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="14" style="0" width="11.76"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -318,7 +334,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -341,6 +357,9 @@
       </c>
       <c r="L1" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -348,105 +367,120 @@
         <f aca="false">ROW()</f>
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="L2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="M2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <f aca="false">ROW()</f>
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4"/>
       <c r="L3" s="4"/>
+      <c r="M3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <f aca="false">ROW()</f>
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="I4" s="1" t="str">
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="J4" s="1" t="str">
         <f aca="false">$C$2</f>
         <v>a</v>
       </c>
-      <c r="J4" s="1" t="str">
+      <c r="K4" s="1" t="str">
         <f aca="false">$C$3</f>
         <v>as</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <f aca="false">ROW()</f>
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="G5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <f aca="false">ROW()</f>
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="I6" s="1" t="str">
+        <v>21</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="J6" s="1" t="str">
         <f aca="false">$C$5</f>
         <v>aas</v>
       </c>
-      <c r="J6" s="1" t="str">
+      <c r="K6" s="1" t="str">
         <f aca="false">$C$4</f>
         <v>aa</v>
       </c>
@@ -456,22 +490,25 @@
         <f aca="false">ROW()</f>
         <v>7</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="I7" s="1" t="str">
+      <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="J7" s="1" t="str">
         <f aca="false">$C$5</f>
         <v>aas</v>
       </c>
-      <c r="J7" s="1" t="str">
+      <c r="K7" s="1" t="str">
         <f aca="false">$C$4</f>
         <v>aa</v>
       </c>
@@ -481,22 +518,25 @@
         <f aca="false">ROW()</f>
         <v>8</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="I8" s="1" t="str">
+      <c r="F8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="J8" s="1" t="str">
         <f aca="false">$C$5</f>
         <v>aas</v>
       </c>
-      <c r="J8" s="1" t="str">
+      <c r="K8" s="1" t="str">
         <f aca="false">$C$4</f>
         <v>aa</v>
       </c>
@@ -1299,286 +1339,6 @@
     <row r="804" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="805" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="806" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>

</xml_diff>